<commit_message>
New data for app
</commit_message>
<xml_diff>
--- a/data/small/admins.xlsx
+++ b/data/small/admins.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\layo\Desktop\ALX\schub\data2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\layo\Desktop\schub\data2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B64C191-C3F8-4106-94F8-3E5EA05A8982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F44B4CF-1410-4401-A2F9-3D34E665AA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{CEEE0883-0B3F-4224-B1DA-2D3DDD7CAC7A}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{CEEE0883-0B3F-4224-B1DA-2D3DDD7CAC7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>2017-03-25 02:17:06</t>
   </si>
@@ -84,20 +84,41 @@
     <t>recovery_answer</t>
   </si>
   <si>
-    <t>Micoliser(FoolishnessIncarnate)</t>
-  </si>
-  <si>
-    <t>FoolishJesulayomi</t>
-  </si>
-  <si>
     <t>What is your baby's name</t>
+  </si>
+  <si>
+    <t>53af4926-52ee-41d0-9acc-ae7230000003</t>
+  </si>
+  <si>
+    <t>2017-03-25 02:17:07</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>tester@schub.com</t>
+  </si>
+  <si>
+    <t>testerpwd</t>
+  </si>
+  <si>
+    <t>General Kenobi</t>
+  </si>
+  <si>
+    <t>Hello there?</t>
+  </si>
+  <si>
+    <t>Micoliser</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +130,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -455,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45DF8C7F-4679-4C52-9B05-6CEB32D48996}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,7 +495,7 @@
     <col min="3" max="3" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30" bestFit="1" customWidth="1"/>
   </cols>
@@ -519,10 +546,10 @@
         <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -545,21 +572,47 @@
         <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4"/>
-      <c r="B4" s="1"/>
-      <c r="E4" s="3"/>
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{DD11FA12-515C-4DA1-9A1A-2550AB0BFA81}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{493B8F96-19A9-46D3-9336-785B3D038A27}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{B2EFE120-FFE0-49B8-9A13-60B9258E240A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Homepage structure and design
</commit_message>
<xml_diff>
--- a/data/small/admins.xlsx
+++ b/data/small/admins.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\layo\Desktop\schub\data2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F44B4CF-1410-4401-A2F9-3D34E665AA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E78214-CA69-4C5C-8BCC-C5BC19558B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{CEEE0883-0B3F-4224-B1DA-2D3DDD7CAC7A}"/>
+    <workbookView xWindow="-28320" yWindow="-600" windowWidth="21600" windowHeight="14865" xr2:uid="{CEEE0883-0B3F-4224-B1DA-2D3DDD7CAC7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
-  <si>
-    <t>2017-03-25 02:17:06</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t>Aina</t>
   </si>
@@ -90,15 +87,6 @@
     <t>53af4926-52ee-41d0-9acc-ae7230000003</t>
   </si>
   <si>
-    <t>2017-03-25 02:17:07</t>
-  </si>
-  <si>
-    <t>Beta</t>
-  </si>
-  <si>
-    <t>Tester</t>
-  </si>
-  <si>
     <t>tester@schub.com</t>
   </si>
   <si>
@@ -112,6 +100,72 @@
   </si>
   <si>
     <t>Micoliser</t>
+  </si>
+  <si>
+    <t>53af4926-52ee-41d0-9acc-ae7230000004</t>
+  </si>
+  <si>
+    <t>Alfred</t>
+  </si>
+  <si>
+    <t>Tuva</t>
+  </si>
+  <si>
+    <t>alfred@schub.com</t>
+  </si>
+  <si>
+    <t>alfredpwd</t>
+  </si>
+  <si>
+    <t>53af4926-52ee-41d0-9acc-ae7230000005</t>
+  </si>
+  <si>
+    <t>Martins</t>
+  </si>
+  <si>
+    <t>Ndifon</t>
+  </si>
+  <si>
+    <t>martins@schub.com</t>
+  </si>
+  <si>
+    <t>martinspwd</t>
+  </si>
+  <si>
+    <t>53af4926-52ee-41d0-9acc-ae7230000006</t>
+  </si>
+  <si>
+    <t>2023-03-25 02:17:10</t>
+  </si>
+  <si>
+    <t>2023-03-25 02:17:09</t>
+  </si>
+  <si>
+    <t>2023-03-25 02:17:08</t>
+  </si>
+  <si>
+    <t>2023-03-25 02:17:07</t>
+  </si>
+  <si>
+    <t>2020-03-25 02:17:06</t>
+  </si>
+  <si>
+    <t>Bot</t>
+  </si>
+  <si>
+    <t>Beta-Tester</t>
+  </si>
+  <si>
+    <t>Julien</t>
+  </si>
+  <si>
+    <t>Barbier</t>
+  </si>
+  <si>
+    <t>julien@schub.com</t>
+  </si>
+  <si>
+    <t>julienpwd</t>
   </si>
 </sst>
 </file>
@@ -482,130 +536,205 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45DF8C7F-4679-4C52-9B05-6CEB32D48996}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="G4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5"/>
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -613,6 +742,9 @@
     <hyperlink ref="E2" r:id="rId1" xr:uid="{DD11FA12-515C-4DA1-9A1A-2550AB0BFA81}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{493B8F96-19A9-46D3-9336-785B3D038A27}"/>
     <hyperlink ref="E4" r:id="rId3" xr:uid="{B2EFE120-FFE0-49B8-9A13-60B9258E240A}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{A9E00D42-66D8-40B9-9C53-DA5A7F62819E}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{AADB1D03-C5F2-4E1A-8194-22A2F788DB35}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{4C082707-E215-4C49-B483-389238BF3FD4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>